<commit_message>
Update code to allow selection for sampling method
</commit_message>
<xml_diff>
--- a/output/SAMPLE_INPUT_50snippets.xlsx
+++ b/output/SAMPLE_INPUT_50snippets.xlsx
@@ -481,21 +481,21 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>91</v>
+        <v>49</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>6:11 AM</t>
+          <t>5:50 AM</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>2725.88</v>
+        <v>1467.18</v>
       </c>
       <c r="D3" t="n">
-        <v>2755.88</v>
+        <v>1497.18</v>
       </c>
       <c r="E3" t="n">
-        <v>22.16</v>
+        <v>24.93</v>
       </c>
     </row>
     <row r="4">
@@ -519,21 +519,21 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>6:25 AM</t>
+          <t>6:27 AM</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>3577.16</v>
+        <v>3687.43</v>
       </c>
       <c r="D5" t="n">
-        <v>3607.16</v>
+        <v>3717.43</v>
       </c>
       <c r="E5" t="n">
-        <v>49.37</v>
+        <v>25.2</v>
       </c>
     </row>
     <row r="6">
@@ -557,800 +557,800 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>6:52 AM</t>
+          <t>6:56 AM</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>5193.04</v>
+        <v>5440.89</v>
       </c>
       <c r="D7" t="n">
-        <v>5223.04</v>
+        <v>5470.89</v>
       </c>
       <c r="E7" t="n">
-        <v>71.97</v>
+        <v>108.74</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>182</v>
+        <v>230</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>6:56 AM</t>
+          <t>7:20 AM</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>5440.89</v>
+        <v>6880.786667</v>
       </c>
       <c r="D8" t="n">
-        <v>5470.89</v>
+        <v>6910.786667</v>
       </c>
       <c r="E8" t="n">
-        <v>108.74</v>
+        <v>32.193333</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>230</v>
+        <v>251</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>7:20 AM</t>
+          <t>7:30 AM</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>6880.786667</v>
+        <v>7516.66</v>
       </c>
       <c r="D9" t="n">
-        <v>6910.786667</v>
+        <v>7546.66</v>
       </c>
       <c r="E9" t="n">
-        <v>32.193333</v>
+        <v>27.63</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>239</v>
+        <v>275</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>7:24 AM</t>
+          <t>7:43 AM</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>7146.62</v>
+        <v>8248.530000000001</v>
       </c>
       <c r="D10" t="n">
-        <v>7176.62</v>
+        <v>8278.530000000001</v>
       </c>
       <c r="E10" t="n">
-        <v>32.95</v>
+        <v>21.35</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>251</v>
+        <v>524</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>7:30 AM</t>
+          <t>9:47 AM</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>7516.66</v>
+        <v>15702.116667</v>
       </c>
       <c r="D11" t="n">
-        <v>7546.66</v>
+        <v>15732.116667</v>
       </c>
       <c r="E11" t="n">
-        <v>27.63</v>
+        <v>35.09</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>275</v>
+        <v>550</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>7:43 AM</t>
+          <t>10:00 A</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>8248.530000000001</v>
+        <v>16484</v>
       </c>
       <c r="D12" t="n">
-        <v>8278.530000000001</v>
+        <v>16514</v>
       </c>
       <c r="E12" t="n">
-        <v>21.35</v>
+        <v>26.08</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>331</v>
+        <v>570</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>8:10 AM</t>
+          <t>10:10 A</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>9903.9</v>
+        <v>17087.03</v>
       </c>
       <c r="D13" t="n">
-        <v>9933.9</v>
+        <v>17117.03</v>
       </c>
       <c r="E13" t="n">
-        <v>66.37</v>
+        <v>37.05</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>524</v>
+        <v>993</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>9:47 AM</t>
+          <t>1:41 PM</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>15702.116667</v>
+        <v>29775.52</v>
       </c>
       <c r="D14" t="n">
-        <v>15732.116667</v>
+        <v>29805.52</v>
       </c>
       <c r="E14" t="n">
-        <v>35.09</v>
+        <v>41.35</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>550</v>
+        <v>1016</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>10:00 A</t>
+          <t>1:53 PM</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>16484</v>
+        <v>30454.73</v>
       </c>
       <c r="D15" t="n">
-        <v>16514</v>
+        <v>30484.73</v>
       </c>
       <c r="E15" t="n">
-        <v>26.08</v>
+        <v>24.88</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>570</v>
+        <v>1022</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>10:10 A</t>
+          <t>1:56 PM</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>17087.03</v>
+        <v>30644.296667</v>
       </c>
       <c r="D16" t="n">
-        <v>17117.03</v>
+        <v>30674.296667</v>
       </c>
       <c r="E16" t="n">
-        <v>37.05</v>
+        <v>24.493333</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>993</v>
+        <v>1036</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>1:41 PM</t>
+          <t>2:03 PM</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>29775.52</v>
+        <v>31058.49</v>
       </c>
       <c r="D17" t="n">
-        <v>29805.52</v>
+        <v>31088.49</v>
       </c>
       <c r="E17" t="n">
-        <v>41.35</v>
+        <v>60.24</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1016</v>
+        <v>1086</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>1:53 PM</t>
+          <t>2:28 PM</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>30454.73</v>
+        <v>32575.77</v>
       </c>
       <c r="D18" t="n">
-        <v>30484.73</v>
+        <v>32605.77</v>
       </c>
       <c r="E18" t="n">
-        <v>24.88</v>
+        <v>21.33</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1022</v>
+        <v>1103</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>1:56 PM</t>
+          <t>2:36 PM</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>30644.296667</v>
+        <v>33070.88</v>
       </c>
       <c r="D19" t="n">
-        <v>30674.296667</v>
+        <v>33100.88</v>
       </c>
       <c r="E19" t="n">
-        <v>24.493333</v>
+        <v>25.1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1036</v>
+        <v>1141</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2:03 PM</t>
+          <t>2:55 PM</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>31058.49</v>
+        <v>34219.87</v>
       </c>
       <c r="D20" t="n">
-        <v>31088.49</v>
+        <v>34249.87</v>
       </c>
       <c r="E20" t="n">
-        <v>60.24</v>
+        <v>21.48</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1086</v>
+        <v>1182</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2:28 PM</t>
+          <t>3:16 PM</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>32575.77</v>
+        <v>35455.655</v>
       </c>
       <c r="D21" t="n">
-        <v>32605.77</v>
+        <v>35485.655</v>
       </c>
       <c r="E21" t="n">
-        <v>21.33</v>
+        <v>37.115</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1103</v>
+        <v>1190</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2:36 PM</t>
+          <t>3:20 PM</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>33070.88</v>
+        <v>35678.675</v>
       </c>
       <c r="D22" t="n">
-        <v>33100.88</v>
+        <v>35708.675</v>
       </c>
       <c r="E22" t="n">
-        <v>25.1</v>
+        <v>40.53</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1141</v>
+        <v>1196</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2:55 PM</t>
+          <t>3:23 PM</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>34219.87</v>
+        <v>35858.715</v>
       </c>
       <c r="D23" t="n">
-        <v>34249.87</v>
+        <v>35888.715</v>
       </c>
       <c r="E23" t="n">
-        <v>21.48</v>
+        <v>56.205</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1180</v>
+        <v>1202</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>3:15 PM</t>
+          <t>3:26 PM</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>35378.663333</v>
+        <v>36041.01</v>
       </c>
       <c r="D24" t="n">
-        <v>35408.663333</v>
+        <v>36071.01</v>
       </c>
       <c r="E24" t="n">
-        <v>42.293333</v>
+        <v>24.126667</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1190</v>
+        <v>1209</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>3:20 PM</t>
+          <t>3:29 PM</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>35678.675</v>
+        <v>36244.02</v>
       </c>
       <c r="D25" t="n">
-        <v>35708.675</v>
+        <v>36274.02</v>
       </c>
       <c r="E25" t="n">
-        <v>40.53</v>
+        <v>75.29000000000001</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1200</v>
+        <v>1221</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>3:25 PM</t>
+          <t>3:35 PM</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>35982.38</v>
+        <v>36616.4</v>
       </c>
       <c r="D26" t="n">
-        <v>36012.38</v>
+        <v>36646.4</v>
       </c>
       <c r="E26" t="n">
-        <v>37.86</v>
+        <v>23.47</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1221</v>
+        <v>1227</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>3:35 PM</t>
+          <t>3:39 PM</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>36616.4</v>
+        <v>36808.87</v>
       </c>
       <c r="D27" t="n">
-        <v>36646.4</v>
+        <v>36838.87</v>
       </c>
       <c r="E27" t="n">
-        <v>23.47</v>
+        <v>22.12</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1227</v>
+        <v>1245</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>3:39 PM</t>
+          <t>3:47 PM</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>36808.87</v>
+        <v>37332.09</v>
       </c>
       <c r="D28" t="n">
-        <v>36838.87</v>
+        <v>37362.09</v>
       </c>
       <c r="E28" t="n">
-        <v>22.12</v>
+        <v>193.12</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1245</v>
+        <v>1269</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>3:47 PM</t>
+          <t>3:59 PM</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>37332.09</v>
+        <v>38052.733333</v>
       </c>
       <c r="D29" t="n">
-        <v>37362.09</v>
+        <v>38082.733333</v>
       </c>
       <c r="E29" t="n">
-        <v>193.12</v>
+        <v>20.703333</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>1257</v>
+        <v>1279</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>3:53 PM</t>
+          <t>4:05 PM</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>37684.8</v>
+        <v>38365.04</v>
       </c>
       <c r="D30" t="n">
-        <v>37714.8</v>
+        <v>38395.04</v>
       </c>
       <c r="E30" t="n">
-        <v>36.82</v>
+        <v>31.16</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>1273</v>
+        <v>1288</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>4:02 PM</t>
+          <t>4:09 PM</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>38186.04</v>
+        <v>38622.23</v>
       </c>
       <c r="D31" t="n">
-        <v>38216.04</v>
+        <v>38652.23</v>
       </c>
       <c r="E31" t="n">
-        <v>28.77</v>
+        <v>50.7</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>1280</v>
+        <v>1302</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>4:05 PM</t>
+          <t>4:16 PM</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>38387.28</v>
+        <v>39032.49</v>
       </c>
       <c r="D32" t="n">
-        <v>38417.28</v>
+        <v>39062.49</v>
       </c>
       <c r="E32" t="n">
-        <v>28.405</v>
+        <v>230.5</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1289</v>
+        <v>1308</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>4:09 PM</t>
+          <t>4:19 PM</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>38650.62</v>
+        <v>39217.913333</v>
       </c>
       <c r="D33" t="n">
-        <v>38680.62</v>
+        <v>39247.913333</v>
       </c>
       <c r="E33" t="n">
-        <v>88.59</v>
+        <v>29.03</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1302</v>
+        <v>1315</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>4:16 PM</t>
+          <t>4:22 PM</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>39032.49</v>
+        <v>39427.435</v>
       </c>
       <c r="D34" t="n">
-        <v>39062.49</v>
+        <v>39457.435</v>
       </c>
       <c r="E34" t="n">
-        <v>230.5</v>
+        <v>98.93000000000001</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>1314</v>
+        <v>1323</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>4:22 PM</t>
+          <t>4:26 PM</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>39391.77</v>
+        <v>39677.255</v>
       </c>
       <c r="D35" t="n">
-        <v>39421.77</v>
+        <v>39707.255</v>
       </c>
       <c r="E35" t="n">
-        <v>27.71</v>
+        <v>57.735</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>1323</v>
+        <v>1333</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>4:26 PM</t>
+          <t>4:31 PM</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>39677.255</v>
+        <v>39975.185</v>
       </c>
       <c r="D36" t="n">
-        <v>39707.255</v>
+        <v>40005.185</v>
       </c>
       <c r="E36" t="n">
-        <v>57.735</v>
+        <v>26.385</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>1335</v>
+        <v>1345</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>4:32 PM</t>
+          <t>4:38 PM</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>40027.72</v>
+        <v>40347.76</v>
       </c>
       <c r="D37" t="n">
-        <v>40057.72</v>
+        <v>40377.76</v>
       </c>
       <c r="E37" t="n">
-        <v>47.705</v>
+        <v>94.73999999999999</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>1343</v>
+        <v>1362</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>4:36 PM</t>
+          <t>4:46 PM</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>40265.54</v>
+        <v>40838.935</v>
       </c>
       <c r="D38" t="n">
-        <v>40295.54</v>
+        <v>40868.935</v>
       </c>
       <c r="E38" t="n">
-        <v>30.27</v>
+        <v>104.33</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>1349</v>
+        <v>1369</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>4:39 PM</t>
+          <t>4:49 PM</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>40446.58</v>
+        <v>41046.07</v>
       </c>
       <c r="D39" t="n">
-        <v>40476.58</v>
+        <v>41076.07</v>
       </c>
       <c r="E39" t="n">
-        <v>52.82</v>
+        <v>33.66</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>1357</v>
+        <v>1390</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>4:43 PM</t>
+          <t>5:00 PM</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>40690.25</v>
+        <v>41680.48</v>
       </c>
       <c r="D40" t="n">
-        <v>40720.25</v>
+        <v>41710.48</v>
       </c>
       <c r="E40" t="n">
-        <v>163.16</v>
+        <v>38.76</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>1367</v>
+        <v>1410</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>4:48 PM</t>
+          <t>5:10 PM</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>40993.815</v>
+        <v>42278.335</v>
       </c>
       <c r="D41" t="n">
-        <v>41023.815</v>
+        <v>42308.335</v>
       </c>
       <c r="E41" t="n">
-        <v>30.44</v>
+        <v>44.55</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>1390</v>
+        <v>1417</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>5:00 PM</t>
+          <t>5:13 PM</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>41680.48</v>
+        <v>42486.06</v>
       </c>
       <c r="D42" t="n">
-        <v>41710.48</v>
+        <v>42516.06</v>
       </c>
       <c r="E42" t="n">
-        <v>38.76</v>
+        <v>61.41</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>1414</v>
+        <v>1427</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>5:12 PM</t>
+          <t>5:19 PM</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>42400.085</v>
+        <v>42809.97</v>
       </c>
       <c r="D43" t="n">
-        <v>42430.085</v>
+        <v>42839.97</v>
       </c>
       <c r="E43" t="n">
-        <v>51.73</v>
+        <v>161.82</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>1432</v>
+        <v>1445</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>5:21 PM</t>
+          <t>5:27 PM</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>42943.82</v>
+        <v>43323.345</v>
       </c>
       <c r="D44" t="n">
-        <v>42973.82</v>
+        <v>43353.345</v>
       </c>
       <c r="E44" t="n">
-        <v>31.495</v>
+        <v>29.31</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>1445</v>
+        <v>1451</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>5:27 PM</t>
+          <t>5:30 PM</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>43323.345</v>
+        <v>43516.02</v>
       </c>
       <c r="D45" t="n">
-        <v>43353.345</v>
+        <v>43546.02</v>
       </c>
       <c r="E45" t="n">
-        <v>29.31</v>
+        <v>88.58</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>1451</v>
+        <v>1472</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>5:30 PM</t>
+          <t>5:41 PM</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>43516.02</v>
+        <v>44138.865</v>
       </c>
       <c r="D46" t="n">
-        <v>43546.02</v>
+        <v>44168.865</v>
       </c>
       <c r="E46" t="n">
-        <v>88.58</v>
+        <v>48.69</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>1472</v>
+        <v>1479</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>5:41 PM</t>
+          <t>5:44 PM</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>44138.865</v>
+        <v>44340.68</v>
       </c>
       <c r="D47" t="n">
-        <v>44168.865</v>
+        <v>44370.68</v>
       </c>
       <c r="E47" t="n">
-        <v>48.69</v>
+        <v>49.65</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>1479</v>
+        <v>1492</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>5:44 PM</t>
+          <t>5:51 PM</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>44340.68</v>
+        <v>44738.87</v>
       </c>
       <c r="D48" t="n">
-        <v>44370.68</v>
+        <v>44768.87</v>
       </c>
       <c r="E48" t="n">
-        <v>49.65</v>
+        <v>22.62</v>
       </c>
     </row>
     <row r="49">

</xml_diff>

<commit_message>
Add new TVN samp[ling method, updates to menu, rework logic controlling file processing info.
</commit_message>
<xml_diff>
--- a/output/SAMPLE_INPUT_50snippets.xlsx
+++ b/output/SAMPLE_INPUT_50snippets.xlsx
@@ -500,477 +500,477 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>6:15 AM</t>
+          <t>6:11 AM</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2986.3175</v>
+        <v>2725.88</v>
       </c>
       <c r="D4" t="n">
-        <v>3016.3175</v>
+        <v>2755.88</v>
       </c>
       <c r="E4" t="n">
-        <v>30.9975</v>
+        <v>22.16</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>6:27 AM</t>
+          <t>6:15 AM</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>3687.43</v>
+        <v>2986.3175</v>
       </c>
       <c r="D5" t="n">
-        <v>3717.43</v>
+        <v>3016.3175</v>
       </c>
       <c r="E5" t="n">
-        <v>25.2</v>
+        <v>30.9975</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>6:40 AM</t>
+          <t>6:27 AM</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>4506.15</v>
+        <v>3687.43</v>
       </c>
       <c r="D6" t="n">
-        <v>4536.15</v>
+        <v>3717.43</v>
       </c>
       <c r="E6" t="n">
-        <v>33.81</v>
+        <v>25.2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>182</v>
+        <v>151</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>6:56 AM</t>
+          <t>6:40 AM</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>5440.89</v>
+        <v>4506.15</v>
       </c>
       <c r="D7" t="n">
-        <v>5470.89</v>
+        <v>4536.15</v>
       </c>
       <c r="E7" t="n">
-        <v>108.74</v>
+        <v>33.81</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>230</v>
+        <v>182</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>7:20 AM</t>
+          <t>6:56 AM</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>6880.786667</v>
+        <v>5440.89</v>
       </c>
       <c r="D8" t="n">
-        <v>6910.786667</v>
+        <v>5470.89</v>
       </c>
       <c r="E8" t="n">
-        <v>32.193333</v>
+        <v>108.74</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>251</v>
+        <v>230</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>7:30 AM</t>
+          <t>7:20 AM</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>7516.66</v>
+        <v>6880.786667</v>
       </c>
       <c r="D9" t="n">
-        <v>7546.66</v>
+        <v>6910.786667</v>
       </c>
       <c r="E9" t="n">
-        <v>27.63</v>
+        <v>32.193333</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>275</v>
+        <v>239</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>7:43 AM</t>
+          <t>7:24 AM</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>8248.530000000001</v>
+        <v>7146.62</v>
       </c>
       <c r="D10" t="n">
-        <v>8278.530000000001</v>
+        <v>7176.62</v>
       </c>
       <c r="E10" t="n">
-        <v>21.35</v>
+        <v>32.95</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>524</v>
+        <v>257</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>9:47 AM</t>
+          <t>7:33 AM</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>15702.116667</v>
+        <v>7691.65</v>
       </c>
       <c r="D11" t="n">
-        <v>15732.116667</v>
+        <v>7721.65</v>
       </c>
       <c r="E11" t="n">
-        <v>35.09</v>
+        <v>35.775</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>550</v>
+        <v>331</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>10:00 A</t>
+          <t>8:10 AM</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>16484</v>
+        <v>9903.9</v>
       </c>
       <c r="D12" t="n">
-        <v>16514</v>
+        <v>9933.9</v>
       </c>
       <c r="E12" t="n">
-        <v>26.08</v>
+        <v>66.37</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>570</v>
+        <v>524</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>10:10 A</t>
+          <t>9:47 AM</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>17087.03</v>
+        <v>15702.116667</v>
       </c>
       <c r="D13" t="n">
-        <v>17117.03</v>
+        <v>15732.116667</v>
       </c>
       <c r="E13" t="n">
-        <v>37.05</v>
+        <v>35.09</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>993</v>
+        <v>550</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>1:41 PM</t>
+          <t>10:00 A</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>29775.52</v>
+        <v>16484</v>
       </c>
       <c r="D14" t="n">
-        <v>29805.52</v>
+        <v>16514</v>
       </c>
       <c r="E14" t="n">
-        <v>41.35</v>
+        <v>26.08</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1016</v>
+        <v>570</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>1:53 PM</t>
+          <t>10:10 A</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>30454.73</v>
+        <v>17087.03</v>
       </c>
       <c r="D15" t="n">
-        <v>30484.73</v>
+        <v>17117.03</v>
       </c>
       <c r="E15" t="n">
-        <v>24.88</v>
+        <v>37.05</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1022</v>
+        <v>1016</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>1:56 PM</t>
+          <t>1:53 PM</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>30644.296667</v>
+        <v>30454.73</v>
       </c>
       <c r="D16" t="n">
-        <v>30674.296667</v>
+        <v>30484.73</v>
       </c>
       <c r="E16" t="n">
-        <v>24.493333</v>
+        <v>24.88</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1036</v>
+        <v>1022</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2:03 PM</t>
+          <t>1:56 PM</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>31058.49</v>
+        <v>30644.296667</v>
       </c>
       <c r="D17" t="n">
-        <v>31088.49</v>
+        <v>30674.296667</v>
       </c>
       <c r="E17" t="n">
-        <v>60.24</v>
+        <v>24.493333</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1086</v>
+        <v>1033</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2:28 PM</t>
+          <t>2:01 PM</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>32575.77</v>
+        <v>30974.42</v>
       </c>
       <c r="D18" t="n">
-        <v>32605.77</v>
+        <v>31004.42</v>
       </c>
       <c r="E18" t="n">
-        <v>21.33</v>
+        <v>36.19</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1103</v>
+        <v>1086</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2:36 PM</t>
+          <t>2:28 PM</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>33070.88</v>
+        <v>32575.77</v>
       </c>
       <c r="D19" t="n">
-        <v>33100.88</v>
+        <v>32605.77</v>
       </c>
       <c r="E19" t="n">
-        <v>25.1</v>
+        <v>21.33</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1141</v>
+        <v>1103</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2:55 PM</t>
+          <t>2:36 PM</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>34219.87</v>
+        <v>33070.88</v>
       </c>
       <c r="D20" t="n">
-        <v>34249.87</v>
+        <v>33100.88</v>
       </c>
       <c r="E20" t="n">
-        <v>21.48</v>
+        <v>25.1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1182</v>
+        <v>1141</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>3:16 PM</t>
+          <t>2:55 PM</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>35455.655</v>
+        <v>34219.87</v>
       </c>
       <c r="D21" t="n">
-        <v>35485.655</v>
+        <v>34249.87</v>
       </c>
       <c r="E21" t="n">
-        <v>37.115</v>
+        <v>21.48</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1190</v>
+        <v>1182</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>3:20 PM</t>
+          <t>3:16 PM</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>35678.675</v>
+        <v>35455.655</v>
       </c>
       <c r="D22" t="n">
-        <v>35708.675</v>
+        <v>35485.655</v>
       </c>
       <c r="E22" t="n">
-        <v>40.53</v>
+        <v>37.115</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1196</v>
+        <v>1200</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>3:23 PM</t>
+          <t>3:25 PM</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>35858.715</v>
+        <v>35982.38</v>
       </c>
       <c r="D23" t="n">
-        <v>35888.715</v>
+        <v>36012.38</v>
       </c>
       <c r="E23" t="n">
-        <v>56.205</v>
+        <v>37.86</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1202</v>
+        <v>1214</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>3:26 PM</t>
+          <t>3:32 PM</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>36041.01</v>
+        <v>36391.61</v>
       </c>
       <c r="D24" t="n">
-        <v>36071.01</v>
+        <v>36421.61</v>
       </c>
       <c r="E24" t="n">
-        <v>24.126667</v>
+        <v>96.52</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1209</v>
+        <v>1221</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>3:29 PM</t>
+          <t>3:35 PM</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>36244.02</v>
+        <v>36616.4</v>
       </c>
       <c r="D25" t="n">
-        <v>36274.02</v>
+        <v>36646.4</v>
       </c>
       <c r="E25" t="n">
-        <v>75.29000000000001</v>
+        <v>23.47</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1221</v>
+        <v>1227</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>3:35 PM</t>
+          <t>3:39 PM</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>36616.4</v>
+        <v>36808.87</v>
       </c>
       <c r="D26" t="n">
-        <v>36646.4</v>
+        <v>36838.87</v>
       </c>
       <c r="E26" t="n">
-        <v>23.47</v>
+        <v>22.12</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1227</v>
+        <v>1245</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>3:39 PM</t>
+          <t>3:47 PM</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>36808.87</v>
+        <v>37332.09</v>
       </c>
       <c r="D27" t="n">
-        <v>36838.87</v>
+        <v>37362.09</v>
       </c>
       <c r="E27" t="n">
-        <v>22.12</v>
+        <v>193.12</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1245</v>
+        <v>1257</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>3:47 PM</t>
+          <t>3:53 PM</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>37332.09</v>
+        <v>37684.8</v>
       </c>
       <c r="D28" t="n">
-        <v>37362.09</v>
+        <v>37714.8</v>
       </c>
       <c r="E28" t="n">
-        <v>193.12</v>
+        <v>36.82</v>
       </c>
     </row>
     <row r="29">
@@ -994,192 +994,192 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>4:05 PM</t>
+          <t>4:03 PM</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>38365.04</v>
+        <v>38285.38</v>
       </c>
       <c r="D30" t="n">
-        <v>38395.04</v>
+        <v>38315.38</v>
       </c>
       <c r="E30" t="n">
-        <v>31.16</v>
+        <v>25.395</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>1288</v>
+        <v>1283</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>4:09 PM</t>
+          <t>4:06 PM</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>38622.23</v>
+        <v>38479.19</v>
       </c>
       <c r="D31" t="n">
-        <v>38652.23</v>
+        <v>38509.19</v>
       </c>
       <c r="E31" t="n">
-        <v>50.7</v>
+        <v>51.24</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>1302</v>
+        <v>1297</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>4:16 PM</t>
+          <t>4:13 PM</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>39032.49</v>
+        <v>38885.46</v>
       </c>
       <c r="D32" t="n">
-        <v>39062.49</v>
+        <v>38915.46</v>
       </c>
       <c r="E32" t="n">
-        <v>230.5</v>
+        <v>73.44</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1308</v>
+        <v>1311</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>4:19 PM</t>
+          <t>4:20 PM</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>39217.913333</v>
+        <v>39315.5</v>
       </c>
       <c r="D33" t="n">
-        <v>39247.913333</v>
+        <v>39345.5</v>
       </c>
       <c r="E33" t="n">
-        <v>29.03</v>
+        <v>76.02</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1315</v>
+        <v>1323</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>4:22 PM</t>
+          <t>4:26 PM</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>39427.435</v>
+        <v>39677.255</v>
       </c>
       <c r="D34" t="n">
-        <v>39457.435</v>
+        <v>39707.255</v>
       </c>
       <c r="E34" t="n">
-        <v>98.93000000000001</v>
+        <v>57.735</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>1323</v>
+        <v>1335</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>4:26 PM</t>
+          <t>4:32 PM</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>39677.255</v>
+        <v>40027.72</v>
       </c>
       <c r="D35" t="n">
-        <v>39707.255</v>
+        <v>40057.72</v>
       </c>
       <c r="E35" t="n">
-        <v>57.735</v>
+        <v>47.705</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>1333</v>
+        <v>1341</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>4:31 PM</t>
+          <t>4:35 PM</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>39975.185</v>
+        <v>40209.895</v>
       </c>
       <c r="D36" t="n">
-        <v>40005.185</v>
+        <v>40239.895</v>
       </c>
       <c r="E36" t="n">
-        <v>26.385</v>
+        <v>54.99</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>1345</v>
+        <v>1349</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>4:38 PM</t>
+          <t>4:39 PM</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>40347.76</v>
+        <v>40446.58</v>
       </c>
       <c r="D37" t="n">
-        <v>40377.76</v>
+        <v>40476.58</v>
       </c>
       <c r="E37" t="n">
-        <v>94.73999999999999</v>
+        <v>52.82</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>1362</v>
+        <v>1360</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>4:46 PM</t>
+          <t>4:45 PM</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>40838.935</v>
+        <v>40775.5</v>
       </c>
       <c r="D38" t="n">
-        <v>40868.935</v>
+        <v>40805.5</v>
       </c>
       <c r="E38" t="n">
-        <v>104.33</v>
+        <v>27.96</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>1369</v>
+        <v>1372</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>4:49 PM</t>
+          <t>4:51 PM</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>41046.07</v>
+        <v>41141.465</v>
       </c>
       <c r="D39" t="n">
-        <v>41076.07</v>
+        <v>41171.465</v>
       </c>
       <c r="E39" t="n">
-        <v>33.66</v>
+        <v>98.08</v>
       </c>
     </row>
     <row r="40">
@@ -1203,59 +1203,59 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>1410</v>
+        <v>1412</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>5:10 PM</t>
+          <t>5:11 PM</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>42278.335</v>
+        <v>42334.07</v>
       </c>
       <c r="D41" t="n">
-        <v>42308.335</v>
+        <v>42364.07</v>
       </c>
       <c r="E41" t="n">
-        <v>44.55</v>
+        <v>101.66</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>5:13 PM</t>
+          <t>5:14 PM</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>42486.06</v>
+        <v>42521.595</v>
       </c>
       <c r="D42" t="n">
-        <v>42516.06</v>
+        <v>42551.595</v>
       </c>
       <c r="E42" t="n">
-        <v>61.41</v>
+        <v>25.965</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>1427</v>
+        <v>1432</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>5:19 PM</t>
+          <t>5:21 PM</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>42809.97</v>
+        <v>42943.82</v>
       </c>
       <c r="D43" t="n">
-        <v>42839.97</v>
+        <v>42973.82</v>
       </c>
       <c r="E43" t="n">
-        <v>161.82</v>
+        <v>31.495</v>
       </c>
     </row>
     <row r="44">

</xml_diff>

<commit_message>
Fix error handling for bad file extensions
</commit_message>
<xml_diff>
--- a/output/SAMPLE_INPUT_50snippets.xlsx
+++ b/output/SAMPLE_INPUT_50snippets.xlsx
@@ -462,116 +462,116 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>5:45 AM</t>
+          <t>5:50 AM</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1169.48</v>
+        <v>1467.18</v>
       </c>
       <c r="D2" t="n">
-        <v>1199.48</v>
+        <v>1497.18</v>
       </c>
       <c r="E2" t="n">
-        <v>21.87</v>
+        <v>24.93</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>49</v>
+        <v>91</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>5:50 AM</t>
+          <t>6:11 AM</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1467.18</v>
+        <v>2725.88</v>
       </c>
       <c r="D3" t="n">
-        <v>1497.18</v>
+        <v>2755.88</v>
       </c>
       <c r="E3" t="n">
-        <v>24.93</v>
+        <v>22.16</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>6:11 AM</t>
+          <t>6:15 AM</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2725.88</v>
+        <v>2986.3175</v>
       </c>
       <c r="D4" t="n">
-        <v>2755.88</v>
+        <v>3016.3175</v>
       </c>
       <c r="E4" t="n">
-        <v>22.16</v>
+        <v>30.9975</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>100</v>
+        <v>123</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>6:15 AM</t>
+          <t>6:27 AM</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2986.3175</v>
+        <v>3687.43</v>
       </c>
       <c r="D5" t="n">
-        <v>3016.3175</v>
+        <v>3717.43</v>
       </c>
       <c r="E5" t="n">
-        <v>30.9975</v>
+        <v>25.2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>123</v>
+        <v>151</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>6:27 AM</t>
+          <t>6:40 AM</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>3687.43</v>
+        <v>4506.15</v>
       </c>
       <c r="D6" t="n">
-        <v>3717.43</v>
+        <v>4536.15</v>
       </c>
       <c r="E6" t="n">
-        <v>25.2</v>
+        <v>33.81</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>151</v>
+        <v>174</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>6:40 AM</t>
+          <t>6:52 AM</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>4506.15</v>
+        <v>5193.04</v>
       </c>
       <c r="D7" t="n">
-        <v>4536.15</v>
+        <v>5223.04</v>
       </c>
       <c r="E7" t="n">
-        <v>33.81</v>
+        <v>71.97</v>
       </c>
     </row>
     <row r="8">
@@ -633,21 +633,21 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>7:33 AM</t>
+          <t>7:30 AM</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>7691.65</v>
+        <v>7516.66</v>
       </c>
       <c r="D11" t="n">
-        <v>7721.65</v>
+        <v>7546.66</v>
       </c>
       <c r="E11" t="n">
-        <v>35.775</v>
+        <v>27.63</v>
       </c>
     </row>
     <row r="12">
@@ -709,21 +709,21 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>570</v>
+        <v>993</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>10:10 A</t>
+          <t>1:41 PM</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>17087.03</v>
+        <v>29775.52</v>
       </c>
       <c r="D15" t="n">
-        <v>17117.03</v>
+        <v>29805.52</v>
       </c>
       <c r="E15" t="n">
-        <v>37.05</v>
+        <v>41.35</v>
       </c>
     </row>
     <row r="16">
@@ -804,97 +804,97 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1103</v>
+        <v>1141</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2:36 PM</t>
+          <t>2:55 PM</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>33070.88</v>
+        <v>34219.87</v>
       </c>
       <c r="D20" t="n">
-        <v>33100.88</v>
+        <v>34249.87</v>
       </c>
       <c r="E20" t="n">
-        <v>25.1</v>
+        <v>21.48</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1141</v>
+        <v>1180</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2:55 PM</t>
+          <t>3:15 PM</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>34219.87</v>
+        <v>35378.663333</v>
       </c>
       <c r="D21" t="n">
-        <v>34249.87</v>
+        <v>35408.663333</v>
       </c>
       <c r="E21" t="n">
-        <v>21.48</v>
+        <v>42.293333</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1182</v>
+        <v>1190</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>3:16 PM</t>
+          <t>3:20 PM</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>35455.655</v>
+        <v>35678.675</v>
       </c>
       <c r="D22" t="n">
-        <v>35485.655</v>
+        <v>35708.675</v>
       </c>
       <c r="E22" t="n">
-        <v>37.115</v>
+        <v>40.53</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1200</v>
+        <v>1196</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>3:25 PM</t>
+          <t>3:23 PM</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>35982.38</v>
+        <v>35858.715</v>
       </c>
       <c r="D23" t="n">
-        <v>36012.38</v>
+        <v>35888.715</v>
       </c>
       <c r="E23" t="n">
-        <v>37.86</v>
+        <v>56.205</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1214</v>
+        <v>1202</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>3:32 PM</t>
+          <t>3:26 PM</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>36391.61</v>
+        <v>36041.01</v>
       </c>
       <c r="D24" t="n">
-        <v>36421.61</v>
+        <v>36071.01</v>
       </c>
       <c r="E24" t="n">
-        <v>96.52</v>
+        <v>24.126667</v>
       </c>
     </row>
     <row r="25">
@@ -1032,268 +1032,268 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>1297</v>
+        <v>1299</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>4:13 PM</t>
+          <t>4:14 PM</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>38885.46</v>
+        <v>38945.82</v>
       </c>
       <c r="D32" t="n">
-        <v>38915.46</v>
+        <v>38975.82</v>
       </c>
       <c r="E32" t="n">
-        <v>73.44</v>
+        <v>32.71</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1311</v>
+        <v>1308</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>4:20 PM</t>
+          <t>4:19 PM</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>39315.5</v>
+        <v>39217.913333</v>
       </c>
       <c r="D33" t="n">
-        <v>39345.5</v>
+        <v>39247.913333</v>
       </c>
       <c r="E33" t="n">
-        <v>76.02</v>
+        <v>29.03</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1323</v>
+        <v>1315</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>4:26 PM</t>
+          <t>4:22 PM</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>39677.255</v>
+        <v>39427.435</v>
       </c>
       <c r="D34" t="n">
-        <v>39707.255</v>
+        <v>39457.435</v>
       </c>
       <c r="E34" t="n">
-        <v>57.735</v>
+        <v>98.93000000000001</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>1335</v>
+        <v>1323</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>4:32 PM</t>
+          <t>4:26 PM</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>40027.72</v>
+        <v>39677.255</v>
       </c>
       <c r="D35" t="n">
-        <v>40057.72</v>
+        <v>39707.255</v>
       </c>
       <c r="E35" t="n">
-        <v>47.705</v>
+        <v>57.735</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>1341</v>
+        <v>1335</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>4:35 PM</t>
+          <t>4:32 PM</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>40209.895</v>
+        <v>40027.72</v>
       </c>
       <c r="D36" t="n">
-        <v>40239.895</v>
+        <v>40057.72</v>
       </c>
       <c r="E36" t="n">
-        <v>54.99</v>
+        <v>47.705</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>1349</v>
+        <v>1343</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>4:39 PM</t>
+          <t>4:36 PM</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>40446.58</v>
+        <v>40265.54</v>
       </c>
       <c r="D37" t="n">
-        <v>40476.58</v>
+        <v>40295.54</v>
       </c>
       <c r="E37" t="n">
-        <v>52.82</v>
+        <v>30.27</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>1360</v>
+        <v>1354</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>4:45 PM</t>
+          <t>4:42 PM</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>40775.5</v>
+        <v>40599.6</v>
       </c>
       <c r="D38" t="n">
-        <v>40805.5</v>
+        <v>40629.6</v>
       </c>
       <c r="E38" t="n">
-        <v>27.96</v>
+        <v>20.99</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>1372</v>
+        <v>1362</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>4:51 PM</t>
+          <t>4:46 PM</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>41141.465</v>
+        <v>40838.935</v>
       </c>
       <c r="D39" t="n">
-        <v>41171.465</v>
+        <v>40868.935</v>
       </c>
       <c r="E39" t="n">
-        <v>98.08</v>
+        <v>104.33</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>1390</v>
+        <v>1372</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>5:00 PM</t>
+          <t>4:51 PM</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>41680.48</v>
+        <v>41141.465</v>
       </c>
       <c r="D40" t="n">
-        <v>41710.48</v>
+        <v>41171.465</v>
       </c>
       <c r="E40" t="n">
-        <v>38.76</v>
+        <v>98.08</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>1412</v>
+        <v>1390</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>5:11 PM</t>
+          <t>5:00 PM</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>42334.07</v>
+        <v>41680.48</v>
       </c>
       <c r="D41" t="n">
-        <v>42364.07</v>
+        <v>41710.48</v>
       </c>
       <c r="E41" t="n">
-        <v>101.66</v>
+        <v>38.76</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>1418</v>
+        <v>1408</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>5:14 PM</t>
+          <t>5:09 PM</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>42521.595</v>
+        <v>42222.19</v>
       </c>
       <c r="D42" t="n">
-        <v>42551.595</v>
+        <v>42252.19</v>
       </c>
       <c r="E42" t="n">
-        <v>25.965</v>
+        <v>25.425</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>1432</v>
+        <v>1418</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>5:21 PM</t>
+          <t>5:14 PM</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>42943.82</v>
+        <v>42521.595</v>
       </c>
       <c r="D43" t="n">
-        <v>42973.82</v>
+        <v>42551.595</v>
       </c>
       <c r="E43" t="n">
-        <v>31.495</v>
+        <v>25.965</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>1445</v>
+        <v>1427</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>5:27 PM</t>
+          <t>5:19 PM</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>43323.345</v>
+        <v>42809.97</v>
       </c>
       <c r="D44" t="n">
-        <v>43353.345</v>
+        <v>42839.97</v>
       </c>
       <c r="E44" t="n">
-        <v>29.31</v>
+        <v>161.82</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>1451</v>
+        <v>1441</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>5:30 PM</t>
+          <t>5:26 PM</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>43516.02</v>
+        <v>43229.93</v>
       </c>
       <c r="D45" t="n">
-        <v>43546.02</v>
+        <v>43259.93</v>
       </c>
       <c r="E45" t="n">
-        <v>88.58</v>
+        <v>24.11</v>
       </c>
     </row>
     <row r="46">
@@ -1393,21 +1393,21 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>1546</v>
+        <v>1551</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>6:18 PM</t>
+          <t>6:20 PM</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>46356.505</v>
+        <v>46502.28</v>
       </c>
       <c r="D51" t="n">
-        <v>46386.505</v>
+        <v>46532.28</v>
       </c>
       <c r="E51" t="n">
-        <v>25.355</v>
+        <v>39.27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Expand sample size if can't find 50 snippets, better error handling
</commit_message>
<xml_diff>
--- a/output/SAMPLE_INPUT_50snippets.xlsx
+++ b/output/SAMPLE_INPUT_50snippets.xlsx
@@ -462,21 +462,21 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>5:50 AM</t>
+          <t>5:45 AM</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1467.18</v>
+        <v>1169.48</v>
       </c>
       <c r="D2" t="n">
-        <v>1497.18</v>
+        <v>1199.48</v>
       </c>
       <c r="E2" t="n">
-        <v>24.93</v>
+        <v>21.87</v>
       </c>
     </row>
     <row r="3">
@@ -519,21 +519,21 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>6:27 AM</t>
+          <t>6:25 AM</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>3687.43</v>
+        <v>3577.16</v>
       </c>
       <c r="D5" t="n">
-        <v>3717.43</v>
+        <v>3607.16</v>
       </c>
       <c r="E5" t="n">
-        <v>25.2</v>
+        <v>49.37</v>
       </c>
     </row>
     <row r="6">
@@ -652,515 +652,515 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>331</v>
+        <v>275</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>8:10 AM</t>
+          <t>7:43 AM</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>9903.9</v>
+        <v>8248.530000000001</v>
       </c>
       <c r="D12" t="n">
-        <v>9933.9</v>
+        <v>8278.530000000001</v>
       </c>
       <c r="E12" t="n">
-        <v>66.37</v>
+        <v>21.35</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>524</v>
+        <v>331</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>9:47 AM</t>
+          <t>8:10 AM</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>15702.116667</v>
+        <v>9903.9</v>
       </c>
       <c r="D13" t="n">
-        <v>15732.116667</v>
+        <v>9933.9</v>
       </c>
       <c r="E13" t="n">
-        <v>35.09</v>
+        <v>66.37</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>550</v>
+        <v>524</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>10:00 A</t>
+          <t>9:47 AM</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>16484</v>
+        <v>15702.116667</v>
       </c>
       <c r="D14" t="n">
-        <v>16514</v>
+        <v>15732.116667</v>
       </c>
       <c r="E14" t="n">
-        <v>26.08</v>
+        <v>35.09</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>993</v>
+        <v>550</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>1:41 PM</t>
+          <t>10:00 A</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>29775.52</v>
+        <v>16484</v>
       </c>
       <c r="D15" t="n">
-        <v>29805.52</v>
+        <v>16514</v>
       </c>
       <c r="E15" t="n">
-        <v>41.35</v>
+        <v>26.08</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1016</v>
+        <v>570</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>1:53 PM</t>
+          <t>10:10 A</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>30454.73</v>
+        <v>17087.03</v>
       </c>
       <c r="D16" t="n">
-        <v>30484.73</v>
+        <v>17117.03</v>
       </c>
       <c r="E16" t="n">
-        <v>24.88</v>
+        <v>37.05</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1022</v>
+        <v>993</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>1:56 PM</t>
+          <t>1:41 PM</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>30644.296667</v>
+        <v>29775.52</v>
       </c>
       <c r="D17" t="n">
-        <v>30674.296667</v>
+        <v>29805.52</v>
       </c>
       <c r="E17" t="n">
-        <v>24.493333</v>
+        <v>41.35</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1033</v>
+        <v>1016</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2:01 PM</t>
+          <t>1:53 PM</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>30974.42</v>
+        <v>30454.73</v>
       </c>
       <c r="D18" t="n">
-        <v>31004.42</v>
+        <v>30484.73</v>
       </c>
       <c r="E18" t="n">
-        <v>36.19</v>
+        <v>24.88</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1086</v>
+        <v>1022</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2:28 PM</t>
+          <t>1:56 PM</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>32575.77</v>
+        <v>30644.296667</v>
       </c>
       <c r="D19" t="n">
-        <v>32605.77</v>
+        <v>30674.296667</v>
       </c>
       <c r="E19" t="n">
-        <v>21.33</v>
+        <v>24.493333</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1141</v>
+        <v>1036</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2:55 PM</t>
+          <t>2:03 PM</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>34219.87</v>
+        <v>31058.49</v>
       </c>
       <c r="D20" t="n">
-        <v>34249.87</v>
+        <v>31088.49</v>
       </c>
       <c r="E20" t="n">
-        <v>21.48</v>
+        <v>60.24</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1180</v>
+        <v>1086</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>3:15 PM</t>
+          <t>2:28 PM</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>35378.663333</v>
+        <v>32575.77</v>
       </c>
       <c r="D21" t="n">
-        <v>35408.663333</v>
+        <v>32605.77</v>
       </c>
       <c r="E21" t="n">
-        <v>42.293333</v>
+        <v>21.33</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1190</v>
+        <v>1103</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>3:20 PM</t>
+          <t>2:36 PM</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>35678.675</v>
+        <v>33070.88</v>
       </c>
       <c r="D22" t="n">
-        <v>35708.675</v>
+        <v>33100.88</v>
       </c>
       <c r="E22" t="n">
-        <v>40.53</v>
+        <v>25.1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1196</v>
+        <v>1141</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>3:23 PM</t>
+          <t>2:55 PM</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>35858.715</v>
+        <v>34219.87</v>
       </c>
       <c r="D23" t="n">
-        <v>35888.715</v>
+        <v>34249.87</v>
       </c>
       <c r="E23" t="n">
-        <v>56.205</v>
+        <v>21.48</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1202</v>
+        <v>1185</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>3:26 PM</t>
+          <t>3:17 PM</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>36041.01</v>
+        <v>35530.52</v>
       </c>
       <c r="D24" t="n">
-        <v>36071.01</v>
+        <v>35560.52</v>
       </c>
       <c r="E24" t="n">
-        <v>24.126667</v>
+        <v>115.925</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1221</v>
+        <v>1196</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>3:35 PM</t>
+          <t>3:23 PM</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>36616.4</v>
+        <v>35858.715</v>
       </c>
       <c r="D25" t="n">
-        <v>36646.4</v>
+        <v>35888.715</v>
       </c>
       <c r="E25" t="n">
-        <v>23.47</v>
+        <v>56.205</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1227</v>
+        <v>1202</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>3:39 PM</t>
+          <t>3:26 PM</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>36808.87</v>
+        <v>36041.01</v>
       </c>
       <c r="D26" t="n">
-        <v>36838.87</v>
+        <v>36071.01</v>
       </c>
       <c r="E26" t="n">
-        <v>22.12</v>
+        <v>24.126667</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1245</v>
+        <v>1209</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>3:47 PM</t>
+          <t>3:29 PM</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>37332.09</v>
+        <v>36244.02</v>
       </c>
       <c r="D27" t="n">
-        <v>37362.09</v>
+        <v>36274.02</v>
       </c>
       <c r="E27" t="n">
-        <v>193.12</v>
+        <v>75.29000000000001</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1257</v>
+        <v>1221</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>3:53 PM</t>
+          <t>3:35 PM</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>37684.8</v>
+        <v>36616.4</v>
       </c>
       <c r="D28" t="n">
-        <v>37714.8</v>
+        <v>36646.4</v>
       </c>
       <c r="E28" t="n">
-        <v>36.82</v>
+        <v>23.47</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1269</v>
+        <v>1227</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>3:59 PM</t>
+          <t>3:39 PM</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>38052.733333</v>
+        <v>36808.87</v>
       </c>
       <c r="D29" t="n">
-        <v>38082.733333</v>
+        <v>36838.87</v>
       </c>
       <c r="E29" t="n">
-        <v>20.703333</v>
+        <v>22.12</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>1277</v>
+        <v>1245</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>4:03 PM</t>
+          <t>3:47 PM</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>38285.38</v>
+        <v>37332.09</v>
       </c>
       <c r="D30" t="n">
-        <v>38315.38</v>
+        <v>37362.09</v>
       </c>
       <c r="E30" t="n">
-        <v>25.395</v>
+        <v>193.12</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>1283</v>
+        <v>1257</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>4:06 PM</t>
+          <t>3:53 PM</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>38479.19</v>
+        <v>37684.8</v>
       </c>
       <c r="D31" t="n">
-        <v>38509.19</v>
+        <v>37714.8</v>
       </c>
       <c r="E31" t="n">
-        <v>51.24</v>
+        <v>36.82</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>1299</v>
+        <v>1273</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>4:14 PM</t>
+          <t>4:02 PM</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>38945.82</v>
+        <v>38186.04</v>
       </c>
       <c r="D32" t="n">
-        <v>38975.82</v>
+        <v>38216.04</v>
       </c>
       <c r="E32" t="n">
-        <v>32.71</v>
+        <v>28.77</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1308</v>
+        <v>1280</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>4:19 PM</t>
+          <t>4:05 PM</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>39217.913333</v>
+        <v>38387.28</v>
       </c>
       <c r="D33" t="n">
-        <v>39247.913333</v>
+        <v>38417.28</v>
       </c>
       <c r="E33" t="n">
-        <v>29.03</v>
+        <v>28.405</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1315</v>
+        <v>1291</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>4:22 PM</t>
+          <t>4:11 PM</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>39427.435</v>
+        <v>38728.38</v>
       </c>
       <c r="D34" t="n">
-        <v>39457.435</v>
+        <v>38758.38</v>
       </c>
       <c r="E34" t="n">
-        <v>98.93000000000001</v>
+        <v>100.57</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>1323</v>
+        <v>1300</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>4:26 PM</t>
+          <t>4:15 PM</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>39677.255</v>
+        <v>38978.615</v>
       </c>
       <c r="D35" t="n">
-        <v>39707.255</v>
+        <v>39008.615</v>
       </c>
       <c r="E35" t="n">
-        <v>57.735</v>
+        <v>27.355</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>1335</v>
+        <v>1314</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>4:32 PM</t>
+          <t>4:22 PM</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>40027.72</v>
+        <v>39391.77</v>
       </c>
       <c r="D36" t="n">
-        <v>40057.72</v>
+        <v>39421.77</v>
       </c>
       <c r="E36" t="n">
-        <v>47.705</v>
+        <v>27.71</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>1343</v>
+        <v>1333</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>4:36 PM</t>
+          <t>4:31 PM</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>40265.54</v>
+        <v>39975.185</v>
       </c>
       <c r="D37" t="n">
-        <v>40295.54</v>
+        <v>40005.185</v>
       </c>
       <c r="E37" t="n">
-        <v>30.27</v>
+        <v>26.385</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>1354</v>
+        <v>1343</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>4:42 PM</t>
+          <t>4:36 PM</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>40599.6</v>
+        <v>40265.54</v>
       </c>
       <c r="D38" t="n">
-        <v>40629.6</v>
+        <v>40295.54</v>
       </c>
       <c r="E38" t="n">
-        <v>20.99</v>
+        <v>30.27</v>
       </c>
     </row>
     <row r="39">
@@ -1184,21 +1184,21 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>1372</v>
+        <v>1369</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>4:51 PM</t>
+          <t>4:49 PM</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>41141.465</v>
+        <v>41046.07</v>
       </c>
       <c r="D40" t="n">
-        <v>41171.465</v>
+        <v>41076.07</v>
       </c>
       <c r="E40" t="n">
-        <v>98.08</v>
+        <v>33.66</v>
       </c>
     </row>
     <row r="41">
@@ -1222,21 +1222,21 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>1408</v>
+        <v>1412</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>5:09 PM</t>
+          <t>5:11 PM</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>42222.19</v>
+        <v>42334.07</v>
       </c>
       <c r="D42" t="n">
-        <v>42252.19</v>
+        <v>42364.07</v>
       </c>
       <c r="E42" t="n">
-        <v>25.425</v>
+        <v>101.66</v>
       </c>
     </row>
     <row r="43">
@@ -1279,97 +1279,97 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>1441</v>
+        <v>1445</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>5:26 PM</t>
+          <t>5:27 PM</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>43229.93</v>
+        <v>43323.345</v>
       </c>
       <c r="D45" t="n">
-        <v>43259.93</v>
+        <v>43353.345</v>
       </c>
       <c r="E45" t="n">
-        <v>24.11</v>
+        <v>29.31</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>1472</v>
+        <v>1451</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>5:41 PM</t>
+          <t>5:30 PM</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>44138.865</v>
+        <v>43516.02</v>
       </c>
       <c r="D46" t="n">
-        <v>44168.865</v>
+        <v>43546.02</v>
       </c>
       <c r="E46" t="n">
-        <v>48.69</v>
+        <v>88.58</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>1479</v>
+        <v>1472</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>5:44 PM</t>
+          <t>5:41 PM</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>44340.68</v>
+        <v>44138.865</v>
       </c>
       <c r="D47" t="n">
-        <v>44370.68</v>
+        <v>44168.865</v>
       </c>
       <c r="E47" t="n">
-        <v>49.65</v>
+        <v>48.69</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>1492</v>
+        <v>1479</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>5:51 PM</t>
+          <t>5:44 PM</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>44738.87</v>
+        <v>44340.68</v>
       </c>
       <c r="D48" t="n">
-        <v>44768.87</v>
+        <v>44370.68</v>
       </c>
       <c r="E48" t="n">
-        <v>22.62</v>
+        <v>49.65</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>1516</v>
+        <v>1492</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>6:03 PM</t>
+          <t>5:51 PM</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>45455.86</v>
+        <v>44738.87</v>
       </c>
       <c r="D49" t="n">
-        <v>45485.86</v>
+        <v>44768.87</v>
       </c>
       <c r="E49" t="n">
-        <v>28.36</v>
+        <v>22.62</v>
       </c>
     </row>
     <row r="50">

</xml_diff>

<commit_message>
Change top 100 to top 50 with time filtering, minor UI changes
</commit_message>
<xml_diff>
--- a/output/SAMPLE_INPUT_50snippets.xlsx
+++ b/output/SAMPLE_INPUT_50snippets.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,16 @@
           <t>AWC</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>TVN</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>CTC</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -478,860 +488,1136 @@
       <c r="E2" t="n">
         <v>21.87</v>
       </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>91</v>
+        <v>49</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>6:11 AM</t>
+          <t>5:50 AM</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>2725.88</v>
+        <v>1467.18</v>
       </c>
       <c r="D3" t="n">
-        <v>2755.88</v>
+        <v>1497.18</v>
       </c>
       <c r="E3" t="n">
-        <v>22.16</v>
+        <v>24.93</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>6:15 AM</t>
+          <t>6:11 AM</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2986.3175</v>
+        <v>2725.88</v>
       </c>
       <c r="D4" t="n">
-        <v>3016.3175</v>
+        <v>2755.88</v>
       </c>
       <c r="E4" t="n">
-        <v>30.9975</v>
+        <v>22.16</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>6:25 AM</t>
+          <t>6:15 AM</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>3577.16</v>
+        <v>2986.3175</v>
       </c>
       <c r="D5" t="n">
-        <v>3607.16</v>
+        <v>3016.3175</v>
       </c>
       <c r="E5" t="n">
-        <v>49.37</v>
+        <v>30.9975</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1.25</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>151</v>
+        <v>120</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>6:40 AM</t>
+          <t>6:25 AM</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>4506.15</v>
+        <v>3577.16</v>
       </c>
       <c r="D6" t="n">
-        <v>4536.15</v>
+        <v>3607.16</v>
       </c>
       <c r="E6" t="n">
-        <v>33.81</v>
+        <v>49.37</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>174</v>
+        <v>151</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>6:52 AM</t>
+          <t>6:40 AM</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>5193.04</v>
+        <v>4506.15</v>
       </c>
       <c r="D7" t="n">
-        <v>5223.04</v>
+        <v>4536.15</v>
       </c>
       <c r="E7" t="n">
-        <v>71.97</v>
+        <v>33.81</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>6:56 AM</t>
+          <t>6:52 AM</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>5440.89</v>
+        <v>5193.04</v>
       </c>
       <c r="D8" t="n">
-        <v>5470.89</v>
+        <v>5223.04</v>
       </c>
       <c r="E8" t="n">
-        <v>108.74</v>
+        <v>71.97</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>230</v>
+        <v>182</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>7:20 AM</t>
+          <t>6:56 AM</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>6880.786667</v>
+        <v>5440.89</v>
       </c>
       <c r="D9" t="n">
-        <v>6910.786667</v>
+        <v>5470.89</v>
       </c>
       <c r="E9" t="n">
-        <v>32.193333</v>
+        <v>108.74</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>7:24 AM</t>
+          <t>7:20 AM</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>7146.62</v>
+        <v>6880.786667</v>
       </c>
       <c r="D10" t="n">
-        <v>7176.62</v>
+        <v>6910.786667</v>
       </c>
       <c r="E10" t="n">
-        <v>32.95</v>
+        <v>32.193333</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1.333333</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>7:30 AM</t>
+          <t>7:24 AM</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>7516.66</v>
+        <v>7146.62</v>
       </c>
       <c r="D11" t="n">
-        <v>7546.66</v>
+        <v>7176.62</v>
       </c>
       <c r="E11" t="n">
-        <v>27.63</v>
+        <v>32.95</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>275</v>
+        <v>257</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>7:43 AM</t>
+          <t>7:33 AM</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>8248.530000000001</v>
+        <v>7691.65</v>
       </c>
       <c r="D12" t="n">
-        <v>8278.530000000001</v>
+        <v>7721.65</v>
       </c>
       <c r="E12" t="n">
-        <v>21.35</v>
+        <v>35.775</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>331</v>
+        <v>275</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>8:10 AM</t>
+          <t>7:43 AM</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>9903.9</v>
+        <v>8248.530000000001</v>
       </c>
       <c r="D13" t="n">
-        <v>9933.9</v>
+        <v>8278.530000000001</v>
       </c>
       <c r="E13" t="n">
-        <v>66.37</v>
+        <v>21.35</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>524</v>
+        <v>331</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>9:47 AM</t>
+          <t>8:10 AM</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>15702.116667</v>
+        <v>9903.9</v>
       </c>
       <c r="D14" t="n">
-        <v>15732.116667</v>
+        <v>9933.9</v>
       </c>
       <c r="E14" t="n">
-        <v>35.09</v>
+        <v>66.37</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>550</v>
+        <v>524</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>10:00 A</t>
+          <t>9:47 AM</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>16484</v>
+        <v>15702.116667</v>
       </c>
       <c r="D15" t="n">
-        <v>16514</v>
+        <v>15732.116667</v>
       </c>
       <c r="E15" t="n">
-        <v>26.08</v>
+        <v>35.09</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>570</v>
+        <v>550</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>10:10 A</t>
+          <t>10:00 A</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>17087.03</v>
+        <v>16484</v>
       </c>
       <c r="D16" t="n">
-        <v>17117.03</v>
+        <v>16514</v>
       </c>
       <c r="E16" t="n">
-        <v>37.05</v>
+        <v>26.08</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>993</v>
+        <v>570</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>1:41 PM</t>
+          <t>10:10 A</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>29775.52</v>
+        <v>17087.03</v>
       </c>
       <c r="D17" t="n">
-        <v>29805.52</v>
+        <v>17117.03</v>
       </c>
       <c r="E17" t="n">
-        <v>41.35</v>
+        <v>37.05</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1016</v>
+        <v>993</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>1:53 PM</t>
+          <t>1:41 PM</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>30454.73</v>
+        <v>29775.52</v>
       </c>
       <c r="D18" t="n">
-        <v>30484.73</v>
+        <v>29805.52</v>
       </c>
       <c r="E18" t="n">
-        <v>24.88</v>
+        <v>41.35</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1022</v>
+        <v>1016</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>1:56 PM</t>
+          <t>1:53 PM</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>30644.296667</v>
+        <v>30454.73</v>
       </c>
       <c r="D19" t="n">
-        <v>30674.296667</v>
+        <v>30484.73</v>
       </c>
       <c r="E19" t="n">
-        <v>24.493333</v>
+        <v>24.88</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1036</v>
+        <v>1027</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2:03 PM</t>
+          <t>1:59 PM</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>31058.49</v>
+        <v>30807.17</v>
       </c>
       <c r="D20" t="n">
-        <v>31088.49</v>
+        <v>30837.17</v>
       </c>
       <c r="E20" t="n">
-        <v>60.24</v>
+        <v>20.12</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1086</v>
+        <v>1036</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2:28 PM</t>
+          <t>2:03 PM</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>32575.77</v>
+        <v>31058.49</v>
       </c>
       <c r="D21" t="n">
-        <v>32605.77</v>
+        <v>31088.49</v>
       </c>
       <c r="E21" t="n">
-        <v>21.33</v>
+        <v>60.24</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1103</v>
+        <v>1078</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2:36 PM</t>
+          <t>2:24 PM</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>33070.88</v>
+        <v>32329.13</v>
       </c>
       <c r="D22" t="n">
-        <v>33100.88</v>
+        <v>32359.13</v>
       </c>
       <c r="E22" t="n">
-        <v>25.1</v>
+        <v>18.55</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1141</v>
+        <v>1086</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2:55 PM</t>
+          <t>2:28 PM</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>34219.87</v>
+        <v>32575.77</v>
       </c>
       <c r="D23" t="n">
-        <v>34249.87</v>
+        <v>32605.77</v>
       </c>
       <c r="E23" t="n">
-        <v>21.48</v>
+        <v>21.33</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1185</v>
+        <v>1103</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>3:17 PM</t>
+          <t>2:36 PM</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>35530.52</v>
+        <v>33070.88</v>
       </c>
       <c r="D24" t="n">
-        <v>35560.52</v>
+        <v>33100.88</v>
       </c>
       <c r="E24" t="n">
-        <v>115.925</v>
+        <v>25.1</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1196</v>
+        <v>1141</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>3:23 PM</t>
+          <t>2:55 PM</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>35858.715</v>
+        <v>34219.87</v>
       </c>
       <c r="D25" t="n">
-        <v>35888.715</v>
+        <v>34249.87</v>
       </c>
       <c r="E25" t="n">
-        <v>56.205</v>
+        <v>21.48</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1202</v>
+        <v>1185</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>3:26 PM</t>
+          <t>3:17 PM</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>36041.01</v>
+        <v>35530.52</v>
       </c>
       <c r="D26" t="n">
-        <v>36071.01</v>
+        <v>35560.52</v>
       </c>
       <c r="E26" t="n">
-        <v>24.126667</v>
+        <v>115.925</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1209</v>
+        <v>1196</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>3:29 PM</t>
+          <t>3:23 PM</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>36244.02</v>
+        <v>35858.715</v>
       </c>
       <c r="D27" t="n">
-        <v>36274.02</v>
+        <v>35888.715</v>
       </c>
       <c r="E27" t="n">
-        <v>75.29000000000001</v>
+        <v>56.205</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1221</v>
+        <v>1204</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>3:35 PM</t>
+          <t>3:27 PM</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>36616.4</v>
+        <v>36097.916667</v>
       </c>
       <c r="D28" t="n">
-        <v>36646.4</v>
+        <v>36127.916667</v>
       </c>
       <c r="E28" t="n">
-        <v>23.47</v>
+        <v>82.06</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1.333333</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1227</v>
+        <v>1214</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>3:39 PM</t>
+          <t>3:32 PM</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>36808.87</v>
+        <v>36391.61</v>
       </c>
       <c r="D29" t="n">
-        <v>36838.87</v>
+        <v>36421.61</v>
       </c>
       <c r="E29" t="n">
-        <v>22.12</v>
+        <v>96.52</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>1245</v>
+        <v>1221</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>3:47 PM</t>
+          <t>3:35 PM</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>37332.09</v>
+        <v>36616.4</v>
       </c>
       <c r="D30" t="n">
-        <v>37362.09</v>
+        <v>36646.4</v>
       </c>
       <c r="E30" t="n">
-        <v>193.12</v>
+        <v>23.47</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>1257</v>
+        <v>1245</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>3:53 PM</t>
+          <t>3:47 PM</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>37684.8</v>
+        <v>37332.09</v>
       </c>
       <c r="D31" t="n">
-        <v>37714.8</v>
+        <v>37362.09</v>
       </c>
       <c r="E31" t="n">
-        <v>36.82</v>
+        <v>193.12</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>1273</v>
+        <v>1257</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>4:02 PM</t>
+          <t>3:53 PM</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>38186.04</v>
+        <v>37684.8</v>
       </c>
       <c r="D32" t="n">
-        <v>38216.04</v>
+        <v>37714.8</v>
       </c>
       <c r="E32" t="n">
-        <v>28.77</v>
+        <v>36.82</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1280</v>
+        <v>1273</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>4:05 PM</t>
+          <t>4:02 PM</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>38387.28</v>
+        <v>38186.04</v>
       </c>
       <c r="D33" t="n">
-        <v>38417.28</v>
+        <v>38216.04</v>
       </c>
       <c r="E33" t="n">
-        <v>28.405</v>
+        <v>28.77</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1291</v>
+        <v>1283</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>4:11 PM</t>
+          <t>4:06 PM</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>38728.38</v>
+        <v>38479.19</v>
       </c>
       <c r="D34" t="n">
-        <v>38758.38</v>
+        <v>38509.19</v>
       </c>
       <c r="E34" t="n">
-        <v>100.57</v>
+        <v>51.24</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>1300</v>
+        <v>1291</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>4:15 PM</t>
+          <t>4:11 PM</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>38978.615</v>
+        <v>38728.38</v>
       </c>
       <c r="D35" t="n">
-        <v>39008.615</v>
+        <v>38758.38</v>
       </c>
       <c r="E35" t="n">
-        <v>27.355</v>
+        <v>100.57</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>1314</v>
+        <v>1302</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>4:22 PM</t>
+          <t>4:16 PM</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>39391.77</v>
+        <v>39032.49</v>
       </c>
       <c r="D36" t="n">
-        <v>39421.77</v>
+        <v>39062.49</v>
       </c>
       <c r="E36" t="n">
-        <v>27.71</v>
+        <v>230.5</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>1333</v>
+        <v>1311</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>4:31 PM</t>
+          <t>4:20 PM</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>39975.185</v>
+        <v>39315.5</v>
       </c>
       <c r="D37" t="n">
-        <v>40005.185</v>
+        <v>39345.5</v>
       </c>
       <c r="E37" t="n">
-        <v>26.385</v>
+        <v>76.02</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" t="n">
+        <v>1.5</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>1343</v>
+        <v>1318</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>4:36 PM</t>
+          <t>4:24 PM</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>40265.54</v>
+        <v>39526.18</v>
       </c>
       <c r="D38" t="n">
-        <v>40295.54</v>
+        <v>39556.18</v>
       </c>
       <c r="E38" t="n">
-        <v>30.27</v>
+        <v>111.31</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" t="n">
+        <v>2.5</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>1362</v>
+        <v>1335</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>4:46 PM</t>
+          <t>4:32 PM</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>40838.935</v>
+        <v>40027.72</v>
       </c>
       <c r="D39" t="n">
-        <v>40868.935</v>
+        <v>40057.72</v>
       </c>
       <c r="E39" t="n">
-        <v>104.33</v>
+        <v>47.705</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>1369</v>
+        <v>1345</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>4:49 PM</t>
+          <t>4:38 PM</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>41046.07</v>
+        <v>40347.76</v>
       </c>
       <c r="D40" t="n">
-        <v>41076.07</v>
+        <v>40377.76</v>
       </c>
       <c r="E40" t="n">
-        <v>33.66</v>
+        <v>94.73999999999999</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>1390</v>
+        <v>1357</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>5:00 PM</t>
+          <t>4:43 PM</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>41680.48</v>
+        <v>40690.25</v>
       </c>
       <c r="D41" t="n">
-        <v>41710.48</v>
+        <v>40720.25</v>
       </c>
       <c r="E41" t="n">
-        <v>38.76</v>
+        <v>163.16</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>1412</v>
+        <v>1372</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>5:11 PM</t>
+          <t>4:51 PM</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>42334.07</v>
+        <v>41141.465</v>
       </c>
       <c r="D42" t="n">
-        <v>42364.07</v>
+        <v>41171.465</v>
       </c>
       <c r="E42" t="n">
-        <v>101.66</v>
+        <v>98.08</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>1418</v>
+        <v>1391</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>5:14 PM</t>
+          <t>5:01 PM</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>42521.595</v>
+        <v>41726.28</v>
       </c>
       <c r="D43" t="n">
-        <v>42551.595</v>
+        <v>41756.28</v>
       </c>
       <c r="E43" t="n">
-        <v>25.965</v>
+        <v>40.32</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>1427</v>
+        <v>1412</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>5:19 PM</t>
+          <t>5:11 PM</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>42809.97</v>
+        <v>42334.07</v>
       </c>
       <c r="D44" t="n">
-        <v>42839.97</v>
+        <v>42364.07</v>
       </c>
       <c r="E44" t="n">
-        <v>161.82</v>
+        <v>101.66</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>1445</v>
+        <v>1427</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>5:27 PM</t>
+          <t>5:19 PM</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>43323.345</v>
+        <v>42809.97</v>
       </c>
       <c r="D45" t="n">
-        <v>43353.345</v>
+        <v>42839.97</v>
       </c>
       <c r="E45" t="n">
-        <v>29.31</v>
+        <v>161.82</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>1451</v>
+        <v>1441</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>5:30 PM</t>
+          <t>5:26 PM</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>43516.02</v>
+        <v>43229.93</v>
       </c>
       <c r="D46" t="n">
-        <v>43546.02</v>
+        <v>43259.93</v>
       </c>
       <c r="E46" t="n">
-        <v>88.58</v>
+        <v>24.11</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>1472</v>
+        <v>1451</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>5:41 PM</t>
+          <t>5:30 PM</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>44138.865</v>
+        <v>43516.02</v>
       </c>
       <c r="D47" t="n">
-        <v>44168.865</v>
+        <v>43546.02</v>
       </c>
       <c r="E47" t="n">
-        <v>48.69</v>
+        <v>88.58</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="48">
@@ -1352,6 +1638,12 @@
       <c r="E48" t="n">
         <v>49.65</v>
       </c>
+      <c r="F48" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -1371,6 +1663,12 @@
       <c r="E49" t="n">
         <v>22.62</v>
       </c>
+      <c r="F49" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -1390,6 +1688,12 @@
       <c r="E50" t="n">
         <v>33.28</v>
       </c>
+      <c r="F50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -1408,6 +1712,12 @@
       </c>
       <c r="E51" t="n">
         <v>39.27</v>
+      </c>
+      <c r="F51" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="G51" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>